<commit_message>
Feature for removing rows added
</commit_message>
<xml_diff>
--- a/LstMetadataprofiltest_formatted.xlsx
+++ b/LstMetadataprofiltest_formatted.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git_Repositories\Freelancing\Abdul_Rehman\deliverable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git_Repositories\Freelancing\Abdul_Rehman_Geo_Souls\Task 2\Excel-to-HTML-Python-script\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="503">
   <si>
     <t xml:space="preserve">Elementnr  </t>
   </si>
@@ -1538,6 +1538,9 @@
   </si>
   <si>
     <t>Innebär att det finns ett defaultvärde som föreslås (som kan ändras)</t>
+  </si>
+  <si>
+    <t>Remove_Rows</t>
   </si>
 </sst>
 </file>
@@ -2348,13 +2351,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL291"/>
+  <dimension ref="A1:BM291"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BK280" workbookViewId="0">
+      <selection activeCell="BM285" sqref="BM285"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="62" max="62" width="155.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="86" customWidth="1"/>
+    <col min="65" max="65" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2520,8 +2531,11 @@
       <c r="BJ1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="AC2" t="s">
         <v>51</v>
       </c>
@@ -2565,7 +2579,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -2576,7 +2590,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2683,7 +2697,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="BK5" t="s">
         <v>67</v>
       </c>
@@ -2691,7 +2705,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2777,7 +2791,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.1</v>
       </c>
@@ -2872,7 +2886,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.2000000000000002</v>
       </c>
@@ -2958,7 +2972,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65" ht="195" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2.2999999999999998</v>
       </c>
@@ -3056,7 +3070,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.4</v>
       </c>
@@ -3151,7 +3165,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -3216,7 +3230,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -3293,7 +3307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4.0999999999999996</v>
       </c>
@@ -3388,7 +3402,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4.2</v>
       </c>
@@ -3477,7 +3491,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:62" ht="270" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -7087,7 +7101,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="87" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:62" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>225</v>
       </c>
@@ -7402,7 +7416,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="93" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:62" ht="60" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>14.4</v>
       </c>
@@ -7493,7 +7507,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="95" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:62" ht="300" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>248</v>
       </c>
@@ -10001,7 +10015,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="183" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:62" ht="345" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>27</v>
       </c>
@@ -10673,7 +10687,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="205" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:62" ht="210" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>378</v>
       </c>
@@ -12221,7 +12235,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="262" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:61" ht="135" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>44</v>
       </c>
@@ -12436,7 +12450,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="267" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:61" ht="120" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>44</v>
       </c>
@@ -12740,7 +12754,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>44</v>
       </c>
@@ -12769,7 +12783,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="274" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>41.1</v>
       </c>
@@ -12816,7 +12830,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="275" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>41.2</v>
       </c>
@@ -12866,7 +12880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="276" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>41.3</v>
       </c>
@@ -12916,7 +12930,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="277" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>41.4</v>
       </c>
@@ -12966,60 +12980,69 @@
         <v>460</v>
       </c>
     </row>
-    <row r="278" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="281" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="282" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="283" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="284" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="285" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="287" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BM285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="288" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>185</v>
       </c>
       <c r="B290" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="BM290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>500</v>
       </c>
       <c r="B291" t="s">
         <v>501</v>
+      </c>
+      <c r="BM291">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>